<commit_message>
update read file excel in appyTestCase.java
</commit_message>
<xml_diff>
--- a/data-test-book-your-femo-here.xlsx
+++ b/data-test-book-your-femo-here.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyencaocuong/auto_test/DemoAuto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FA109196-9DC9-4842-B68D-36C762BE3BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A980CEF-7D46-1041-B0C5-F221F072E845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="16660" xr2:uid="{5DAA04CD-6B78-C84A-9039-58F007407E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Element" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -471,7 +472,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,8 +664,8 @@
       <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="1">
-        <v>987654321</v>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -709,4 +710,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B13AAE-E93A-154D-B3BE-33D4A935C118}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update read file excel in HappyTestCase.java
</commit_message>
<xml_diff>
--- a/data-test-book-your-femo-here.xlsx
+++ b/data-test-book-your-femo-here.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyencaocuong/auto_test/DemoAuto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A980CEF-7D46-1041-B0C5-F221F072E845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD461CC-8B82-564F-8B7A-67C1E7373370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="16660" xr2:uid="{5DAA04CD-6B78-C84A-9039-58F007407E7D}"/>
+    <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="16660" activeTab="1" xr2:uid="{5DAA04CD-6B78-C84A-9039-58F007407E7D}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
   <si>
     <t>email</t>
   </si>
@@ -82,6 +82,69 @@
   </si>
   <si>
     <t>This is the test content</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>xpath=./ancestor::div[contains(@class,'mktoFieldWrap')]/div[contains(@class,'mktoError')]</t>
+  </si>
+  <si>
+    <t>checkbox</t>
+  </si>
+  <si>
+    <t>xpath=//div[contains(@class,'mktoCheckboxList')]//input</t>
+  </si>
+  <si>
+    <t>id=Email</t>
+  </si>
+  <si>
+    <t>btnSubmit</t>
+  </si>
+  <si>
+    <t>css=button.mktoButton</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>id=FirstName</t>
+  </si>
+  <si>
+    <t>id=LastName</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>id=Phone</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>id=Country</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>id=Company</t>
+  </si>
+  <si>
+    <t>id=Solution_Interest__c</t>
+  </si>
+  <si>
+    <t>selectInterest</t>
+  </si>
+  <si>
+    <t>id=Sales_Contact_Comments__c</t>
+  </si>
+  <si>
+    <t>areaComment</t>
   </si>
 </sst>
 </file>
@@ -471,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D76DBF-B8F0-B848-B0EF-5A8214B8A358}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,12 +777,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B13AAE-E93A-154D-B3BE-33D4A935C118}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove code Assert and move from @Test to @BeforeMethod
</commit_message>
<xml_diff>
--- a/data-test-book-your-femo-here.xlsx
+++ b/data-test-book-your-femo-here.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyencaocuong/auto_test/DemoAuto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD461CC-8B82-564F-8B7A-67C1E7373370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110C18B8-B4A4-214B-BEBC-F900265AABCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="600" windowWidth="28040" windowHeight="16660" activeTab="1" xr2:uid="{5DAA04CD-6B78-C84A-9039-58F007407E7D}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D76DBF-B8F0-B848-B0EF-5A8214B8A358}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B13AAE-E93A-154D-B3BE-33D4A935C118}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>